<commit_message>
merge chartInFreeze into chart.aul
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/chart.xlsx
+++ b/src/main/webapp/WEB-INF/books/chart.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A49A6EC-C66A-FF48-9704-CA9FAAC0AB9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="20115" windowHeight="9270"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="20120" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chart" sheetId="1" r:id="rId1"/>
+    <sheet name="freeze" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="RangeMerged">#REF!</definedName>
+    <definedName name="TestRange1">#REF!</definedName>
+    <definedName name="TestRange2">#REF!</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Chrome</t>
   </si>
@@ -33,18 +45,29 @@
   <si>
     <t>Safari</t>
   </si>
+  <si>
+    <t>Browser market share 2013</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -68,83 +91,227 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PIE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="75"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>freeze!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Chrome</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Internet Explorer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Firefox</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Others</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Opera</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Safari</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>freeze!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>44.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.170000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.07</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-58E5-4A41-9EA2-29E7EE0BF77F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.70019920318725093"/>
+          <c:y val="0.18529458333168791"/>
+          <c:w val="0.25885988970479812"/>
+          <c:h val="0.61298011477378889"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="4 Gráfico">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7BEDFCA-387F-8C46-B9B9-FAADE6EB5815}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -155,7 +322,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -190,7 +357,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,9 +389,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,6 +441,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -431,16 +634,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +654,7 @@
         <v>44.6</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -456,7 +662,7 @@
         <v>22.08</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -464,7 +670,7 @@
         <v>18.170000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -472,7 +678,7 @@
         <v>9.07</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -480,7 +686,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -491,4 +697,76 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11046E2C-26A0-CA4D-8305-08A7FD002019}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>44.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>22.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>18.170000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>9.07</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>3.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>